<commit_message>
All da Power in PowerPoint ;)
</commit_message>
<xml_diff>
--- a/PowerTable.xlsx
+++ b/PowerTable.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Troel\Dropbox\Kandidat\Wireless\Wireless-Sensor-Networks\Wireless-Sensor-Networks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -91,7 +91,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -186,19 +186,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -277,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -292,12 +279,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -624,7 +609,7 @@
   <dimension ref="B1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="B2" sqref="B2:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,13 +622,13 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="39.75" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="18"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="16"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -680,12 +665,12 @@
       <c r="E4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="9">
-        <v>176.47909999999999</v>
+      <c r="F4" s="10">
+        <v>176.48230000000001</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -697,12 +682,12 @@
       <c r="E5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="11">
-        <v>176.48310000000001</v>
+      <c r="F5" s="10">
+        <v>176.52119999999999</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -714,12 +699,12 @@
       <c r="E6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="12">
-        <v>13083</v>
+      <c r="F6" s="10">
+        <v>13101</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="10">
+      <c r="B7" s="9">
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -731,12 +716,12 @@
       <c r="E7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="12">
-        <v>13106</v>
+      <c r="F7" s="10">
+        <v>13319</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="10">
+      <c r="B8" s="9">
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -748,25 +733,25 @@
       <c r="E8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="12">
-        <v>796.24990000000003</v>
+      <c r="F8" s="10">
+        <v>796.31690000000003</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="13">
+      <c r="B9" s="11">
         <v>6</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="15">
-        <v>796.33339999999998</v>
+      <c r="F9" s="13">
+        <v>797.11419999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>